<commit_message>
Inserido calculo e exibição do drawdown máximo da estratégia
</commit_message>
<xml_diff>
--- a/spread_mm.xlsx
+++ b/spread_mm.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>3677.091607591685</v>
+        <v>3218.075183923917</v>
       </c>
     </row>
     <row r="7">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.7354183215183371</v>
+        <v>0.6436150367847835</v>
       </c>
     </row>
     <row r="8">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -610,7 +610,7 @@
         <v>-1.49380956377302</v>
       </c>
       <c r="J2" t="n">
-        <v>18.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -648,7 +648,7 @@
         <v>-1.055238905407133</v>
       </c>
       <c r="J3" t="n">
-        <v>18.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -686,7 +686,7 @@
         <v>-1.4009522937593</v>
       </c>
       <c r="J4" t="n">
-        <v>18.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -724,7 +724,7 @@
         <v>-1.20904758998326</v>
       </c>
       <c r="J5" t="n">
-        <v>18.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -762,7 +762,7 @@
         <v>-1.57095191592262</v>
       </c>
       <c r="J6" t="n">
-        <v>18.07999992370605</v>
+        <v>17.60000038146973</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>-1.575714202154252</v>
       </c>
       <c r="J7" t="n">
-        <v>18.07999992370605</v>
+        <v>17.60000038146973</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -838,13 +838,13 @@
         <v>-1.243333453223819</v>
       </c>
       <c r="J8" t="n">
-        <v>18.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>17.73999977111816</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>39.45867853853225</v>
       </c>
     </row>
     <row r="9">
@@ -876,7 +876,7 @@
         <v>-1.086667287917365</v>
       </c>
       <c r="J9" t="n">
-        <v>18.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -914,7 +914,7 @@
         <v>-1.11142839704241</v>
       </c>
       <c r="J10" t="n">
-        <v>18.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -952,7 +952,7 @@
         <v>-1.051905495779856</v>
       </c>
       <c r="J11" t="n">
-        <v>18.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -1031,10 +1031,10 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>18.10000038146973</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>5.524988216063184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1066,7 +1066,7 @@
         <v>-0.7880943843296606</v>
       </c>
       <c r="J14" t="n">
-        <v>17.6200008392334</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1104,7 +1104,7 @@
         <v>-0.9804764702206583</v>
       </c>
       <c r="J15" t="n">
-        <v>17.6200008392334</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -1142,7 +1142,7 @@
         <v>-1.04380989074707</v>
       </c>
       <c r="J16" t="n">
-        <v>17.6200008392334</v>
+        <v>0</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -1180,7 +1180,7 @@
         <v>-1.11857069106329</v>
       </c>
       <c r="J17" t="n">
-        <v>17.6200008392334</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
@@ -1218,7 +1218,7 @@
         <v>-1.19476218450637</v>
       </c>
       <c r="J18" t="n">
-        <v>17.6200008392334</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
@@ -1256,7 +1256,7 @@
         <v>-0.9914291018531429</v>
       </c>
       <c r="J19" t="n">
-        <v>17.6200008392334</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
@@ -1294,7 +1294,7 @@
         <v>-1.059999375116256</v>
       </c>
       <c r="J20" t="n">
-        <v>17.6200008392334</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
@@ -1370,7 +1370,7 @@
         <v>-0.9838094257173076</v>
       </c>
       <c r="J22" t="n">
-        <v>17.6200008392334</v>
+        <v>0</v>
       </c>
       <c r="K22" t="n">
         <v>0</v>
@@ -1408,7 +1408,7 @@
         <v>-0.8514289855957031</v>
       </c>
       <c r="J23" t="n">
-        <v>17.6200008392334</v>
+        <v>0</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
@@ -1449,10 +1449,10 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>18.04999923706055</v>
+        <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>119.1131346266954</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2206,7 +2206,7 @@
         <v>-0.8585725511823377</v>
       </c>
       <c r="J44" t="n">
-        <v>17.70999908447266</v>
+        <v>0</v>
       </c>
       <c r="K44" t="n">
         <v>0</v>
@@ -2247,10 +2247,10 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>17.79999923706055</v>
+        <v>0</v>
       </c>
       <c r="L45" t="n">
-        <v>25.28094282175741</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -2282,7 +2282,7 @@
         <v>-1.111427942911785</v>
       </c>
       <c r="J46" t="n">
-        <v>17.3700008392334</v>
+        <v>0</v>
       </c>
       <c r="K46" t="n">
         <v>0</v>
@@ -2323,10 +2323,10 @@
         <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>18.14999961853027</v>
+        <v>0</v>
       </c>
       <c r="L47" t="n">
-        <v>214.8757012921736</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2472,7 +2472,7 @@
         <v>-1.045238585699174</v>
       </c>
       <c r="J51" t="n">
-        <v>17.22999954223633</v>
+        <v>0</v>
       </c>
       <c r="K51" t="n">
         <v>0</v>
@@ -2513,10 +2513,10 @@
         <v>0</v>
       </c>
       <c r="K52" t="n">
-        <v>17.70000076293945</v>
+        <v>0</v>
       </c>
       <c r="L52" t="n">
-        <v>132.7687006904602</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2548,7 +2548,7 @@
         <v>-0.9423809051513672</v>
       </c>
       <c r="J53" t="n">
-        <v>17.17000007629395</v>
+        <v>0</v>
       </c>
       <c r="K53" t="n">
         <v>0</v>
@@ -2589,10 +2589,10 @@
         <v>0</v>
       </c>
       <c r="K54" t="n">
-        <v>17.81999969482422</v>
+        <v>0</v>
       </c>
       <c r="L54" t="n">
-        <v>182.3792451351906</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -3878,7 +3878,7 @@
         <v>-1.007142657325382</v>
       </c>
       <c r="J88" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K88" t="n">
         <v>0</v>
@@ -3916,7 +3916,7 @@
         <v>-0.8995245978945761</v>
       </c>
       <c r="J89" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K89" t="n">
         <v>0</v>
@@ -3954,7 +3954,7 @@
         <v>-1.181427910214378</v>
       </c>
       <c r="J90" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K90" t="n">
         <v>0</v>
@@ -3992,7 +3992,7 @@
         <v>-1.526189713251021</v>
       </c>
       <c r="J91" t="n">
-        <v>18.84000015258789</v>
+        <v>18.1200008392334</v>
       </c>
       <c r="K91" t="n">
         <v>0</v>
@@ -4030,13 +4030,13 @@
         <v>-0.8104770297095882</v>
       </c>
       <c r="J92" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K92" t="n">
-        <v>0</v>
+        <v>18.79999923706055</v>
       </c>
       <c r="L92" t="n">
-        <v>0</v>
+        <v>180.8506450592465</v>
       </c>
     </row>
     <row r="93">
@@ -4068,7 +4068,7 @@
         <v>-1.202380679902575</v>
       </c>
       <c r="J93" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K93" t="n">
         <v>0</v>
@@ -4106,7 +4106,7 @@
         <v>-1.383333297002885</v>
       </c>
       <c r="J94" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K94" t="n">
         <v>0</v>
@@ -4144,7 +4144,7 @@
         <v>-1.545238313220796</v>
       </c>
       <c r="J95" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K95" t="n">
         <v>0</v>
@@ -4182,7 +4182,7 @@
         <v>-2.032380331130256</v>
       </c>
       <c r="J96" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K96" t="n">
         <v>0</v>
@@ -4220,7 +4220,7 @@
         <v>-2.182381675356911</v>
       </c>
       <c r="J97" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K97" t="n">
         <v>0</v>
@@ -4258,7 +4258,7 @@
         <v>-2.495238349551247</v>
       </c>
       <c r="J98" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K98" t="n">
         <v>0</v>
@@ -4296,7 +4296,7 @@
         <v>-2.807143075125559</v>
       </c>
       <c r="J99" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K99" t="n">
         <v>0</v>
@@ -4334,7 +4334,7 @@
         <v>-2.427142551967076</v>
       </c>
       <c r="J100" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K100" t="n">
         <v>0</v>
@@ -4372,7 +4372,7 @@
         <v>-2.197143282209122</v>
       </c>
       <c r="J101" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K101" t="n">
         <v>0</v>
@@ -4410,7 +4410,7 @@
         <v>-1.792857942127046</v>
       </c>
       <c r="J102" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K102" t="n">
         <v>0</v>
@@ -4448,7 +4448,7 @@
         <v>-1.827618916829426</v>
       </c>
       <c r="J103" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K103" t="n">
         <v>0</v>
@@ -4486,7 +4486,7 @@
         <v>-1.689999171665736</v>
       </c>
       <c r="J104" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K104" t="n">
         <v>0</v>
@@ -4524,7 +4524,7 @@
         <v>-2.18666630699521</v>
       </c>
       <c r="J105" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K105" t="n">
         <v>0</v>
@@ -4562,7 +4562,7 @@
         <v>-1.478095599583217</v>
       </c>
       <c r="J106" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K106" t="n">
         <v>0</v>
@@ -4600,7 +4600,7 @@
         <v>-1.25333327338809</v>
       </c>
       <c r="J107" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K107" t="n">
         <v>0</v>
@@ -4638,7 +4638,7 @@
         <v>-1.858095623198011</v>
       </c>
       <c r="J108" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K108" t="n">
         <v>0</v>
@@ -4676,7 +4676,7 @@
         <v>-1.825238091605051</v>
       </c>
       <c r="J109" t="n">
-        <v>18.84000015258789</v>
+        <v>17.82999992370605</v>
       </c>
       <c r="K109" t="n">
         <v>0</v>
@@ -4714,7 +4714,7 @@
         <v>-1.402380988711403</v>
       </c>
       <c r="J110" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K110" t="n">
         <v>0</v>
@@ -4752,7 +4752,7 @@
         <v>-0.7604759761265356</v>
       </c>
       <c r="J111" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K111" t="n">
         <v>0</v>
@@ -4790,7 +4790,7 @@
         <v>-0.9623806363060368</v>
       </c>
       <c r="J112" t="n">
-        <v>18.84000015258789</v>
+        <v>0</v>
       </c>
       <c r="K112" t="n">
         <v>0</v>
@@ -5895,10 +5895,10 @@
         <v>0</v>
       </c>
       <c r="K141" t="n">
-        <v>0</v>
+        <v>18.26000022888184</v>
       </c>
       <c r="L141" t="n">
-        <v>0</v>
+        <v>117.7437841691946</v>
       </c>
     </row>
     <row r="142">
@@ -6617,10 +6617,10 @@
         <v>0</v>
       </c>
       <c r="K160" t="n">
-        <v>18.89999961853027</v>
+        <v>0</v>
       </c>
       <c r="L160" t="n">
-        <v>15.87287490830346</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -8400,7 +8400,7 @@
         <v>-1.029047829764231</v>
       </c>
       <c r="J207" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K207" t="n">
         <v>0</v>
@@ -8438,7 +8438,7 @@
         <v>-1.161905561174667</v>
       </c>
       <c r="J208" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K208" t="n">
         <v>0</v>
@@ -8476,7 +8476,7 @@
         <v>-1.413333620343888</v>
       </c>
       <c r="J209" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K209" t="n">
         <v>0</v>
@@ -8514,7 +8514,7 @@
         <v>-0.9257135845365987</v>
       </c>
       <c r="J210" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K210" t="n">
         <v>0</v>
@@ -8552,7 +8552,7 @@
         <v>-2.562380472819012</v>
       </c>
       <c r="J211" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K211" t="n">
         <v>0</v>
@@ -8590,7 +8590,7 @@
         <v>-2.279999869210378</v>
       </c>
       <c r="J212" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K212" t="n">
         <v>0</v>
@@ -8628,7 +8628,7 @@
         <v>-2.215715226672945</v>
       </c>
       <c r="J213" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K213" t="n">
         <v>0</v>
@@ -8666,7 +8666,7 @@
         <v>-1.922381809779576</v>
       </c>
       <c r="J214" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K214" t="n">
         <v>0</v>
@@ -8704,7 +8704,7 @@
         <v>-2.178571882702055</v>
       </c>
       <c r="J215" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K215" t="n">
         <v>0</v>
@@ -8742,7 +8742,7 @@
         <v>-1.817618324643089</v>
       </c>
       <c r="J216" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K216" t="n">
         <v>0</v>
@@ -8780,7 +8780,7 @@
         <v>-1.839048385620117</v>
       </c>
       <c r="J217" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K217" t="n">
         <v>0</v>
@@ -8818,7 +8818,7 @@
         <v>-2.222856521606445</v>
       </c>
       <c r="J218" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K218" t="n">
         <v>0</v>
@@ -8856,7 +8856,7 @@
         <v>-1.989047095889138</v>
       </c>
       <c r="J219" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K219" t="n">
         <v>0</v>
@@ -8894,7 +8894,7 @@
         <v>-1.518096015566872</v>
       </c>
       <c r="J220" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K220" t="n">
         <v>0</v>
@@ -8932,7 +8932,7 @@
         <v>-1.274285634358723</v>
       </c>
       <c r="J221" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K221" t="n">
         <v>0</v>
@@ -8970,7 +8970,7 @@
         <v>-1.640476953415643</v>
       </c>
       <c r="J222" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K222" t="n">
         <v>0</v>
@@ -9008,7 +9008,7 @@
         <v>-1.381428400675457</v>
       </c>
       <c r="J223" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K223" t="n">
         <v>0</v>
@@ -9046,7 +9046,7 @@
         <v>-0.7876190003894621</v>
       </c>
       <c r="J224" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K224" t="n">
         <v>0</v>
@@ -9084,7 +9084,7 @@
         <v>-0.9376191638764872</v>
       </c>
       <c r="J225" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K225" t="n">
         <v>0</v>
@@ -9388,7 +9388,7 @@
         <v>-0.8442857833135697</v>
       </c>
       <c r="J233" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K233" t="n">
         <v>0</v>
@@ -9464,7 +9464,7 @@
         <v>-1.151904968988326</v>
       </c>
       <c r="J235" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K235" t="n">
         <v>0</v>
@@ -9502,7 +9502,7 @@
         <v>-0.8219045457385832</v>
       </c>
       <c r="J236" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K236" t="n">
         <v>0</v>
@@ -9540,7 +9540,7 @@
         <v>-0.9419043404715417</v>
       </c>
       <c r="J237" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K237" t="n">
         <v>0</v>
@@ -9578,7 +9578,7 @@
         <v>-0.9357145400274369</v>
       </c>
       <c r="J238" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K238" t="n">
         <v>0</v>
@@ -9654,7 +9654,7 @@
         <v>-0.9499999000912638</v>
       </c>
       <c r="J240" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K240" t="n">
         <v>0</v>
@@ -9692,7 +9692,7 @@
         <v>-0.9485712959652872</v>
       </c>
       <c r="J241" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K241" t="n">
         <v>0</v>
@@ -9730,7 +9730,7 @@
         <v>-1.175714084080287</v>
       </c>
       <c r="J242" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K242" t="n">
         <v>0</v>
@@ -9768,7 +9768,7 @@
         <v>-0.946190470740909</v>
       </c>
       <c r="J243" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K243" t="n">
         <v>0</v>
@@ -9882,7 +9882,7 @@
         <v>-0.9676188514346151</v>
       </c>
       <c r="J246" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K246" t="n">
         <v>0</v>
@@ -9920,7 +9920,7 @@
         <v>-0.8647624424525677</v>
       </c>
       <c r="J247" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K247" t="n">
         <v>0</v>
@@ -9958,7 +9958,7 @@
         <v>-0.8357142947968974</v>
       </c>
       <c r="J248" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K248" t="n">
         <v>0</v>
@@ -9996,7 +9996,7 @@
         <v>-0.984285717918759</v>
       </c>
       <c r="J249" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K249" t="n">
         <v>0</v>
@@ -10034,7 +10034,7 @@
         <v>-0.9709527606055843</v>
       </c>
       <c r="J250" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K250" t="n">
         <v>0</v>
@@ -10072,7 +10072,7 @@
         <v>-0.8733337039039242</v>
       </c>
       <c r="J251" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K251" t="n">
         <v>0</v>
@@ -10110,7 +10110,7 @@
         <v>-1.597142673674083</v>
       </c>
       <c r="J252" t="n">
-        <v>19.07999992370605</v>
+        <v>17.36000061035156</v>
       </c>
       <c r="K252" t="n">
         <v>0</v>
@@ -10148,7 +10148,7 @@
         <v>-1.236666679382324</v>
       </c>
       <c r="J253" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K253" t="n">
         <v>0</v>
@@ -10186,7 +10186,7 @@
         <v>-1.385714530944824</v>
       </c>
       <c r="J254" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K254" t="n">
         <v>0</v>
@@ -10224,7 +10224,7 @@
         <v>-0.9114286786034</v>
       </c>
       <c r="J255" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K255" t="n">
         <v>0</v>
@@ -10870,7 +10870,7 @@
         <v>-0.9242857070196244</v>
       </c>
       <c r="J272" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K272" t="n">
         <v>0</v>
@@ -10908,7 +10908,7 @@
         <v>-0.7642853600638251</v>
       </c>
       <c r="J273" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K273" t="n">
         <v>0</v>
@@ -10946,7 +10946,7 @@
         <v>-0.8376192819504507</v>
       </c>
       <c r="J274" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K274" t="n">
         <v>0</v>
@@ -10984,7 +10984,7 @@
         <v>-1.108571143377395</v>
       </c>
       <c r="J275" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K275" t="n">
         <v>0</v>
@@ -11022,7 +11022,7 @@
         <v>-0.9561907450358067</v>
       </c>
       <c r="J276" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K276" t="n">
         <v>0</v>
@@ -11098,7 +11098,7 @@
         <v>-0.9071430478777209</v>
       </c>
       <c r="J278" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K278" t="n">
         <v>0</v>
@@ -11136,7 +11136,7 @@
         <v>-1.053333509536017</v>
       </c>
       <c r="J279" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K279" t="n">
         <v>0</v>
@@ -11174,7 +11174,7 @@
         <v>-1.149524007524763</v>
       </c>
       <c r="J280" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K280" t="n">
         <v>0</v>
@@ -12355,10 +12355,10 @@
         <v>0</v>
       </c>
       <c r="K311" t="n">
-        <v>0</v>
+        <v>17.70000076293945</v>
       </c>
       <c r="L311" t="n">
-        <v>0</v>
+        <v>96.04523670411032</v>
       </c>
     </row>
     <row r="312">
@@ -13112,7 +13112,7 @@
         <v>-1.075713838849747</v>
       </c>
       <c r="J331" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K331" t="n">
         <v>0</v>
@@ -13150,7 +13150,7 @@
         <v>-1.160953158424014</v>
       </c>
       <c r="J332" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K332" t="n">
         <v>0</v>
@@ -13188,7 +13188,7 @@
         <v>-0.7790480114164815</v>
       </c>
       <c r="J333" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K333" t="n">
         <v>0</v>
@@ -13226,7 +13226,7 @@
         <v>-1.000952039446151</v>
       </c>
       <c r="J334" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K334" t="n">
         <v>0</v>
@@ -13264,7 +13264,7 @@
         <v>-1.173333667573473</v>
       </c>
       <c r="J335" t="n">
-        <v>19.07999992370605</v>
+        <v>0</v>
       </c>
       <c r="K335" t="n">
         <v>0</v>
@@ -14179,10 +14179,10 @@
         <v>0</v>
       </c>
       <c r="K359" t="n">
-        <v>19.10000038146973</v>
+        <v>0</v>
       </c>
       <c r="L359" t="n">
-        <v>5.235721823093717</v>
+        <v>0</v>
       </c>
     </row>
     <row r="360">
@@ -15012,7 +15012,7 @@
         <v>-1.19904699779692</v>
       </c>
       <c r="J381" t="n">
-        <v>18.69000053405762</v>
+        <v>0</v>
       </c>
       <c r="K381" t="n">
         <v>0</v>
@@ -15050,7 +15050,7 @@
         <v>-1.25523767017183</v>
       </c>
       <c r="J382" t="n">
-        <v>18.69000053405762</v>
+        <v>0</v>
       </c>
       <c r="K382" t="n">
         <v>0</v>
@@ -15091,10 +15091,10 @@
         <v>0</v>
       </c>
       <c r="K383" t="n">
-        <v>20.05999946594238</v>
+        <v>0</v>
       </c>
       <c r="L383" t="n">
-        <v>341.4753161411426</v>
+        <v>0</v>
       </c>
     </row>
     <row r="384">
@@ -15772,7 +15772,7 @@
         <v>-0.8233327411469951</v>
       </c>
       <c r="J401" t="n">
-        <v>20.95000076293945</v>
+        <v>0</v>
       </c>
       <c r="K401" t="n">
         <v>0</v>
@@ -15813,10 +15813,10 @@
         <v>0</v>
       </c>
       <c r="K402" t="n">
-        <v>21.20999908447266</v>
+        <v>0</v>
       </c>
       <c r="L402" t="n">
-        <v>61.29145043753014</v>
+        <v>0</v>
       </c>
     </row>
     <row r="403">
@@ -15886,13 +15886,13 @@
         <v>-1.411428724016464</v>
       </c>
       <c r="J404" t="n">
-        <v>20.13999938964844</v>
+        <v>0</v>
       </c>
       <c r="K404" t="n">
-        <v>0</v>
+        <v>20.57999992370605</v>
       </c>
       <c r="L404" t="n">
-        <v>0</v>
+        <v>106.9000329661765</v>
       </c>
     </row>
     <row r="405">
@@ -15927,10 +15927,10 @@
         <v>0</v>
       </c>
       <c r="K405" t="n">
-        <v>21.54999923706055</v>
+        <v>0</v>
       </c>
       <c r="L405" t="n">
-        <v>327.1461478725406</v>
+        <v>0</v>
       </c>
     </row>
     <row r="406">
@@ -16000,7 +16000,7 @@
         <v>-0.8104753948393331</v>
       </c>
       <c r="J407" t="n">
-        <v>21.29000091552734</v>
+        <v>0</v>
       </c>
       <c r="K407" t="n">
         <v>0</v>
@@ -16038,7 +16038,7 @@
         <v>-1.171905063447497</v>
       </c>
       <c r="J408" t="n">
-        <v>21.29000091552734</v>
+        <v>0</v>
       </c>
       <c r="K408" t="n">
         <v>0</v>
@@ -16076,7 +16076,7 @@
         <v>-1.476190476190474</v>
       </c>
       <c r="J409" t="n">
-        <v>21.29000091552734</v>
+        <v>0</v>
       </c>
       <c r="K409" t="n">
         <v>0</v>
@@ -16114,7 +16114,7 @@
         <v>-1.845239003499348</v>
       </c>
       <c r="J410" t="n">
-        <v>21.29000091552734</v>
+        <v>20.1299991607666</v>
       </c>
       <c r="K410" t="n">
         <v>0</v>
@@ -16152,7 +16152,7 @@
         <v>-1.668571926298597</v>
       </c>
       <c r="J411" t="n">
-        <v>21.29000091552734</v>
+        <v>20.1299991607666</v>
       </c>
       <c r="K411" t="n">
         <v>0</v>
@@ -16190,7 +16190,7 @@
         <v>-1.915714173089889</v>
       </c>
       <c r="J412" t="n">
-        <v>21.29000091552734</v>
+        <v>20.1299991607666</v>
       </c>
       <c r="K412" t="n">
         <v>0</v>
@@ -16231,10 +16231,10 @@
         <v>0</v>
       </c>
       <c r="K413" t="n">
-        <v>0</v>
+        <v>20.94000053405762</v>
       </c>
       <c r="L413" t="n">
-        <v>0</v>
+        <v>193.4100650985177</v>
       </c>
     </row>
     <row r="414">
@@ -16266,7 +16266,7 @@
         <v>-2.838571094331286</v>
       </c>
       <c r="J414" t="n">
-        <v>21.29000091552734</v>
+        <v>18.60000038146973</v>
       </c>
       <c r="K414" t="n">
         <v>0</v>
@@ -16304,7 +16304,7 @@
         <v>-3.075238000778924</v>
       </c>
       <c r="J415" t="n">
-        <v>21.29000091552734</v>
+        <v>18.60000038146973</v>
       </c>
       <c r="K415" t="n">
         <v>0</v>
@@ -16342,7 +16342,7 @@
         <v>-3.719523747762043</v>
       </c>
       <c r="J416" t="n">
-        <v>21.29000091552734</v>
+        <v>18.60000038146973</v>
       </c>
       <c r="K416" t="n">
         <v>0</v>
@@ -16380,7 +16380,7 @@
         <v>-3.192857923961821</v>
       </c>
       <c r="J417" t="n">
-        <v>21.29000091552734</v>
+        <v>18.60000038146973</v>
       </c>
       <c r="K417" t="n">
         <v>0</v>
@@ -16418,7 +16418,7 @@
         <v>-1.931428182692756</v>
       </c>
       <c r="J418" t="n">
-        <v>21.29000091552734</v>
+        <v>18.60000038146973</v>
       </c>
       <c r="K418" t="n">
         <v>0</v>
@@ -16459,10 +16459,10 @@
         <v>0</v>
       </c>
       <c r="K419" t="n">
-        <v>0</v>
+        <v>20.38999938964844</v>
       </c>
       <c r="L419" t="n">
-        <v>0</v>
+        <v>438.9404271114041</v>
       </c>
     </row>
     <row r="420">
@@ -16649,10 +16649,10 @@
         <v>0</v>
       </c>
       <c r="K424" t="n">
-        <v>22.1299991607666</v>
+        <v>0</v>
       </c>
       <c r="L424" t="n">
-        <v>189.7872293480375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="425">
@@ -16760,7 +16760,7 @@
         <v>-1.33047648838588</v>
       </c>
       <c r="J427" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K427" t="n">
         <v>0</v>
@@ -16798,7 +16798,7 @@
         <v>-0.7857140132359106</v>
       </c>
       <c r="J428" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K428" t="n">
         <v>0</v>
@@ -16836,7 +16836,7 @@
         <v>-1.813333148048038</v>
       </c>
       <c r="J429" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K429" t="n">
         <v>0</v>
@@ -16874,7 +16874,7 @@
         <v>-2.657619294666109</v>
       </c>
       <c r="J430" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K430" t="n">
         <v>0</v>
@@ -16912,7 +16912,7 @@
         <v>-2.779999324253627</v>
       </c>
       <c r="J431" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K431" t="n">
         <v>0</v>
@@ -16950,7 +16950,7 @@
         <v>-3.655237833658855</v>
       </c>
       <c r="J432" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K432" t="n">
         <v>0</v>
@@ -16988,7 +16988,7 @@
         <v>-2.391903922671364</v>
       </c>
       <c r="J433" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K433" t="n">
         <v>0</v>
@@ -17026,7 +17026,7 @@
         <v>-4.186190014793759</v>
       </c>
       <c r="J434" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K434" t="n">
         <v>0</v>
@@ -17064,7 +17064,7 @@
         <v>-3.506190708705358</v>
       </c>
       <c r="J435" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K435" t="n">
         <v>0</v>
@@ -17102,7 +17102,7 @@
         <v>-4.322380474635533</v>
       </c>
       <c r="J436" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K436" t="n">
         <v>0</v>
@@ -17140,7 +17140,7 @@
         <v>-3.890476453871955</v>
       </c>
       <c r="J437" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K437" t="n">
         <v>0</v>
@@ -17178,7 +17178,7 @@
         <v>-2.834285963149298</v>
       </c>
       <c r="J438" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K438" t="n">
         <v>0</v>
@@ -17216,7 +17216,7 @@
         <v>-3.097618647984095</v>
       </c>
       <c r="J439" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K439" t="n">
         <v>0</v>
@@ -17254,7 +17254,7 @@
         <v>-2.86238125392369</v>
       </c>
       <c r="J440" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K440" t="n">
         <v>0</v>
@@ -17292,7 +17292,7 @@
         <v>-2.958095641363236</v>
       </c>
       <c r="J441" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K441" t="n">
         <v>0</v>
@@ -17330,7 +17330,7 @@
         <v>-2.974761508759997</v>
       </c>
       <c r="J442" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K442" t="n">
         <v>0</v>
@@ -17368,7 +17368,7 @@
         <v>-2.434761456080846</v>
       </c>
       <c r="J443" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K443" t="n">
         <v>0</v>
@@ -17406,7 +17406,7 @@
         <v>-2.435714767092751</v>
       </c>
       <c r="J444" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K444" t="n">
         <v>0</v>
@@ -17444,7 +17444,7 @@
         <v>-2.028571492149716</v>
       </c>
       <c r="J445" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K445" t="n">
         <v>0</v>
@@ -17482,7 +17482,7 @@
         <v>-1.561905134291877</v>
       </c>
       <c r="J446" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K446" t="n">
         <v>0</v>
@@ -17520,7 +17520,7 @@
         <v>-1.759999683925084</v>
       </c>
       <c r="J447" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K447" t="n">
         <v>0</v>
@@ -17558,7 +17558,7 @@
         <v>-1.900476455688477</v>
       </c>
       <c r="J448" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K448" t="n">
         <v>0</v>
@@ -17596,7 +17596,7 @@
         <v>-2.191428275335403</v>
       </c>
       <c r="J449" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K449" t="n">
         <v>0</v>
@@ -17634,7 +17634,7 @@
         <v>-2.080952644348145</v>
       </c>
       <c r="J450" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K450" t="n">
         <v>0</v>
@@ -17672,7 +17672,7 @@
         <v>-1.554762249901181</v>
       </c>
       <c r="J451" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K451" t="n">
         <v>0</v>
@@ -17900,7 +17900,7 @@
         <v>-1.056666465032668</v>
       </c>
       <c r="J457" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K457" t="n">
         <v>0</v>
@@ -17938,7 +17938,7 @@
         <v>-1.481428827558245</v>
       </c>
       <c r="J458" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K458" t="n">
         <v>0</v>
@@ -17976,7 +17976,7 @@
         <v>-1.483333224341983</v>
       </c>
       <c r="J459" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K459" t="n">
         <v>0</v>
@@ -18014,7 +18014,7 @@
         <v>-0.8414284842354913</v>
       </c>
       <c r="J460" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K460" t="n">
         <v>0</v>
@@ -18052,7 +18052,7 @@
         <v>-1.15999952952067</v>
       </c>
       <c r="J461" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K461" t="n">
         <v>0</v>
@@ -18090,7 +18090,7 @@
         <v>-1.144285429091681</v>
       </c>
       <c r="J462" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K462" t="n">
         <v>0</v>
@@ -18128,7 +18128,7 @@
         <v>-1.692856924874443</v>
       </c>
       <c r="J463" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K463" t="n">
         <v>0</v>
@@ -18166,7 +18166,7 @@
         <v>-1.647142773582821</v>
       </c>
       <c r="J464" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K464" t="n">
         <v>0</v>
@@ -18204,7 +18204,7 @@
         <v>-2.039523715064639</v>
       </c>
       <c r="J465" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K465" t="n">
         <v>0</v>
@@ -18242,7 +18242,7 @@
         <v>-2.129047530038017</v>
       </c>
       <c r="J466" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K466" t="n">
         <v>0</v>
@@ -18280,7 +18280,7 @@
         <v>-2.382381393795921</v>
       </c>
       <c r="J467" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K467" t="n">
         <v>0</v>
@@ -18318,7 +18318,7 @@
         <v>-3.29619008018857</v>
       </c>
       <c r="J468" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K468" t="n">
         <v>0</v>
@@ -18356,7 +18356,7 @@
         <v>-2.80380966549828</v>
       </c>
       <c r="J469" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K469" t="n">
         <v>0</v>
@@ -18394,7 +18394,7 @@
         <v>-2.554761659531366</v>
       </c>
       <c r="J470" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K470" t="n">
         <v>0</v>
@@ -18432,7 +18432,7 @@
         <v>-2.317619369143532</v>
       </c>
       <c r="J471" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K471" t="n">
         <v>0</v>
@@ -18470,7 +18470,7 @@
         <v>-1.917142958868117</v>
       </c>
       <c r="J472" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K472" t="n">
         <v>0</v>
@@ -18508,7 +18508,7 @@
         <v>-1.190000125340053</v>
       </c>
       <c r="J473" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K473" t="n">
         <v>0</v>
@@ -18584,7 +18584,7 @@
         <v>-0.9004765011015401</v>
       </c>
       <c r="J475" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K475" t="n">
         <v>0</v>
@@ -18660,7 +18660,7 @@
         <v>-0.8428574062529073</v>
       </c>
       <c r="J477" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K477" t="n">
         <v>0</v>
@@ -18698,7 +18698,7 @@
         <v>-1.347143173217773</v>
       </c>
       <c r="J478" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K478" t="n">
         <v>0</v>
@@ -18736,7 +18736,7 @@
         <v>-1.968094825744629</v>
       </c>
       <c r="J479" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K479" t="n">
         <v>0</v>
@@ -18774,7 +18774,7 @@
         <v>-2.062857400803338</v>
       </c>
       <c r="J480" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K480" t="n">
         <v>0</v>
@@ -18812,7 +18812,7 @@
         <v>-1.480476106916155</v>
       </c>
       <c r="J481" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K481" t="n">
         <v>0</v>
@@ -18850,7 +18850,7 @@
         <v>-0.7757146926153276</v>
       </c>
       <c r="J482" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K482" t="n">
         <v>0</v>
@@ -18926,7 +18926,7 @@
         <v>-0.9114283607119607</v>
       </c>
       <c r="J484" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K484" t="n">
         <v>0</v>
@@ -19458,7 +19458,7 @@
         <v>-0.9304759615943539</v>
       </c>
       <c r="J498" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K498" t="n">
         <v>0</v>
@@ -20408,7 +20408,7 @@
         <v>-0.8680947167532782</v>
       </c>
       <c r="J523" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K523" t="n">
         <v>0</v>
@@ -20484,7 +20484,7 @@
         <v>-0.8557139805385052</v>
       </c>
       <c r="J525" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K525" t="n">
         <v>0</v>
@@ -20522,7 +20522,7 @@
         <v>-0.9585712523687455</v>
       </c>
       <c r="J526" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K526" t="n">
         <v>0</v>
@@ -20560,7 +20560,7 @@
         <v>-0.8757139387584871</v>
       </c>
       <c r="J527" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K527" t="n">
         <v>0</v>
@@ -22384,7 +22384,7 @@
         <v>-0.9895234789167127</v>
       </c>
       <c r="J575" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K575" t="n">
         <v>0</v>
@@ -22422,7 +22422,7 @@
         <v>-0.8404762177240279</v>
       </c>
       <c r="J576" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K576" t="n">
         <v>0</v>
@@ -22498,7 +22498,7 @@
         <v>-1.021428607759022</v>
       </c>
       <c r="J578" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K578" t="n">
         <v>0</v>
@@ -22536,7 +22536,7 @@
         <v>-0.9580955051240458</v>
       </c>
       <c r="J579" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K579" t="n">
         <v>0</v>
@@ -23334,7 +23334,7 @@
         <v>-0.792857351757231</v>
       </c>
       <c r="J600" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K600" t="n">
         <v>0</v>
@@ -23410,7 +23410,7 @@
         <v>-1.118571281433105</v>
       </c>
       <c r="J602" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K602" t="n">
         <v>0</v>
@@ -23448,7 +23448,7 @@
         <v>-1.31809511638823</v>
       </c>
       <c r="J603" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K603" t="n">
         <v>0</v>
@@ -23486,7 +23486,7 @@
         <v>-1.019999685741606</v>
       </c>
       <c r="J604" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K604" t="n">
         <v>0</v>
@@ -23524,7 +23524,7 @@
         <v>-1.256666773841495</v>
       </c>
       <c r="J605" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K605" t="n">
         <v>0</v>
@@ -23562,7 +23562,7 @@
         <v>-0.8461902255103695</v>
       </c>
       <c r="J606" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K606" t="n">
         <v>0</v>
@@ -23600,7 +23600,7 @@
         <v>-0.8038097109113416</v>
       </c>
       <c r="J607" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K607" t="n">
         <v>0</v>
@@ -23752,7 +23752,7 @@
         <v>-0.9276192528860907</v>
       </c>
       <c r="J611" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K611" t="n">
         <v>0</v>
@@ -23790,7 +23790,7 @@
         <v>-1.420952479044596</v>
       </c>
       <c r="J612" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K612" t="n">
         <v>0</v>
@@ -23828,7 +23828,7 @@
         <v>-1.365714799790155</v>
       </c>
       <c r="J613" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K613" t="n">
         <v>0</v>
@@ -23866,7 +23866,7 @@
         <v>-1.601905141557966</v>
       </c>
       <c r="J614" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K614" t="n">
         <v>0</v>
@@ -23904,7 +23904,7 @@
         <v>-1.70619060879662</v>
       </c>
       <c r="J615" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K615" t="n">
         <v>0</v>
@@ -23942,7 +23942,7 @@
         <v>-1.644285974048433</v>
       </c>
       <c r="J616" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K616" t="n">
         <v>0</v>
@@ -23980,7 +23980,7 @@
         <v>-2.026666641235352</v>
       </c>
       <c r="J617" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K617" t="n">
         <v>0</v>
@@ -24018,7 +24018,7 @@
         <v>-1.354761441548666</v>
       </c>
       <c r="J618" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K618" t="n">
         <v>0</v>
@@ -24170,7 +24170,7 @@
         <v>-0.9442859377179822</v>
       </c>
       <c r="J622" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K622" t="n">
         <v>0</v>
@@ -24246,7 +24246,7 @@
         <v>-0.8166663760230648</v>
       </c>
       <c r="J624" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K624" t="n">
         <v>0</v>
@@ -24322,7 +24322,7 @@
         <v>-0.9842860358101984</v>
       </c>
       <c r="J626" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K626" t="n">
         <v>0</v>
@@ -24474,7 +24474,7 @@
         <v>-0.7895236696515759</v>
       </c>
       <c r="J630" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K630" t="n">
         <v>0</v>
@@ -24512,7 +24512,7 @@
         <v>-0.8614282608032227</v>
       </c>
       <c r="J631" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K631" t="n">
         <v>0</v>
@@ -24550,7 +24550,7 @@
         <v>-0.9038097744896305</v>
       </c>
       <c r="J632" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K632" t="n">
         <v>0</v>
@@ -24588,7 +24588,7 @@
         <v>-0.9780953271048407</v>
       </c>
       <c r="J633" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K633" t="n">
         <v>0</v>
@@ -24626,7 +24626,7 @@
         <v>-1.133333433242072</v>
       </c>
       <c r="J634" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K634" t="n">
         <v>0</v>
@@ -24664,7 +24664,7 @@
         <v>-1.10380981082008</v>
       </c>
       <c r="J635" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K635" t="n">
         <v>0</v>
@@ -24702,7 +24702,7 @@
         <v>-1.407142548334031</v>
       </c>
       <c r="J636" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K636" t="n">
         <v>0</v>
@@ -24740,7 +24740,7 @@
         <v>-1.715238117036366</v>
       </c>
       <c r="J637" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K637" t="n">
         <v>0</v>
@@ -24778,7 +24778,7 @@
         <v>-1.676666645776658</v>
       </c>
       <c r="J638" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K638" t="n">
         <v>0</v>
@@ -24816,7 +24816,7 @@
         <v>-1.306666419619607</v>
       </c>
       <c r="J639" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K639" t="n">
         <v>0</v>
@@ -25234,7 +25234,7 @@
         <v>-0.9595239503043036</v>
       </c>
       <c r="J650" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K650" t="n">
         <v>0</v>
@@ -25272,7 +25272,7 @@
         <v>-0.8147620927719839</v>
       </c>
       <c r="J651" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K651" t="n">
         <v>0</v>
@@ -25310,7 +25310,7 @@
         <v>-0.8061903544834674</v>
       </c>
       <c r="J652" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K652" t="n">
         <v>0</v>
@@ -25462,7 +25462,7 @@
         <v>-0.9338093939281649</v>
       </c>
       <c r="J656" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K656" t="n">
         <v>0</v>
@@ -25500,7 +25500,7 @@
         <v>-1.200476442064558</v>
       </c>
       <c r="J657" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K657" t="n">
         <v>0</v>
@@ -25538,7 +25538,7 @@
         <v>-1.29952369417463</v>
       </c>
       <c r="J658" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K658" t="n">
         <v>0</v>
@@ -25576,7 +25576,7 @@
         <v>-1.117142881665911</v>
       </c>
       <c r="J659" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K659" t="n">
         <v>0</v>
@@ -25614,7 +25614,7 @@
         <v>-1.194761798495339</v>
       </c>
       <c r="J660" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K660" t="n">
         <v>0</v>
@@ -25652,7 +25652,7 @@
         <v>-1.456666673932757</v>
       </c>
       <c r="J661" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K661" t="n">
         <v>0</v>
@@ -25690,7 +25690,7 @@
         <v>-1.190952278318859</v>
       </c>
       <c r="J662" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K662" t="n">
         <v>0</v>
@@ -27818,7 +27818,7 @@
         <v>-0.866190592447917</v>
       </c>
       <c r="J718" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K718" t="n">
         <v>0</v>
@@ -28236,7 +28236,7 @@
         <v>-0.7976188659667969</v>
       </c>
       <c r="J729" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K729" t="n">
         <v>0</v>
@@ -28274,7 +28274,7 @@
         <v>-1.281428337097168</v>
       </c>
       <c r="J730" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K730" t="n">
         <v>0</v>
@@ -28312,7 +28312,7 @@
         <v>-1.428095227196103</v>
       </c>
       <c r="J731" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K731" t="n">
         <v>0</v>
@@ -28350,7 +28350,7 @@
         <v>-0.92428563890003</v>
       </c>
       <c r="J732" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K732" t="n">
         <v>0</v>
@@ -28388,7 +28388,7 @@
         <v>-1.34523800441197</v>
       </c>
       <c r="J733" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K733" t="n">
         <v>0</v>
@@ -28426,7 +28426,7 @@
         <v>-1.600475992475237</v>
       </c>
       <c r="J734" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K734" t="n">
         <v>0</v>
@@ -28464,7 +28464,7 @@
         <v>-1.609047753470285</v>
       </c>
       <c r="J735" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K735" t="n">
         <v>0</v>
@@ -28502,7 +28502,7 @@
         <v>-1.702857289995466</v>
       </c>
       <c r="J736" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K736" t="n">
         <v>0</v>
@@ -28540,7 +28540,7 @@
         <v>-1.504285698845273</v>
       </c>
       <c r="J737" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K737" t="n">
         <v>0</v>
@@ -28578,7 +28578,7 @@
         <v>-1.470000130789621</v>
       </c>
       <c r="J738" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K738" t="n">
         <v>0</v>
@@ -28616,7 +28616,7 @@
         <v>-1.563809690021333</v>
       </c>
       <c r="J739" t="n">
-        <v>18.64999961853027</v>
+        <v>17.92000007629395</v>
       </c>
       <c r="K739" t="n">
         <v>0</v>
@@ -28654,7 +28654,7 @@
         <v>-1.088095051901681</v>
       </c>
       <c r="J740" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K740" t="n">
         <v>0</v>
@@ -28692,7 +28692,7 @@
         <v>-0.9471429416111539</v>
       </c>
       <c r="J741" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K741" t="n">
         <v>0</v>
@@ -28806,7 +28806,7 @@
         <v>-0.9504760106404619</v>
       </c>
       <c r="J744" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K744" t="n">
         <v>0</v>
@@ -31580,7 +31580,7 @@
         <v>-0.8219046365647085</v>
       </c>
       <c r="J817" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K817" t="n">
         <v>0</v>
@@ -31618,7 +31618,7 @@
         <v>-0.8542860121954057</v>
       </c>
       <c r="J818" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K818" t="n">
         <v>0</v>
@@ -31656,7 +31656,7 @@
         <v>-1.194761821201869</v>
       </c>
       <c r="J819" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K819" t="n">
         <v>0</v>
@@ -31694,7 +31694,7 @@
         <v>-1.126666841052828</v>
       </c>
       <c r="J820" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K820" t="n">
         <v>0</v>
@@ -31732,7 +31732,7 @@
         <v>-0.9390474501110262</v>
       </c>
       <c r="J821" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K821" t="n">
         <v>0</v>
@@ -31770,7 +31770,7 @@
         <v>-1.282857486179896</v>
       </c>
       <c r="J822" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K822" t="n">
         <v>0</v>
@@ -31808,7 +31808,7 @@
         <v>-1.044761703127907</v>
       </c>
       <c r="J823" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K823" t="n">
         <v>0</v>
@@ -31846,7 +31846,7 @@
         <v>-1.28047616141183</v>
       </c>
       <c r="J824" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K824" t="n">
         <v>0</v>
@@ -31884,7 +31884,7 @@
         <v>-1.045713924226307</v>
       </c>
       <c r="J825" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K825" t="n">
         <v>0</v>
@@ -31922,7 +31922,7 @@
         <v>-0.8361907232375376</v>
       </c>
       <c r="J826" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K826" t="n">
         <v>0</v>
@@ -35687,10 +35687,10 @@
         <v>0</v>
       </c>
       <c r="K925" t="n">
-        <v>0</v>
+        <v>17.95000076293945</v>
       </c>
       <c r="L925" t="n">
-        <v>0</v>
+        <v>8.356736871969627</v>
       </c>
     </row>
     <row r="926">
@@ -36026,7 +36026,7 @@
         <v>-0.8128575370425253</v>
       </c>
       <c r="J934" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K934" t="n">
         <v>0</v>
@@ -36178,7 +36178,7 @@
         <v>-1.575714429219563</v>
       </c>
       <c r="J938" t="n">
-        <v>18.64999961853027</v>
+        <v>15.5</v>
       </c>
       <c r="K938" t="n">
         <v>0</v>
@@ -36216,7 +36216,7 @@
         <v>-2.999999909173873</v>
       </c>
       <c r="J939" t="n">
-        <v>18.64999961853027</v>
+        <v>15.5</v>
       </c>
       <c r="K939" t="n">
         <v>0</v>
@@ -36254,7 +36254,7 @@
         <v>-2.926190603347052</v>
       </c>
       <c r="J940" t="n">
-        <v>18.64999961853027</v>
+        <v>15.5</v>
       </c>
       <c r="K940" t="n">
         <v>0</v>
@@ -36292,7 +36292,7 @@
         <v>-2.113809858049667</v>
       </c>
       <c r="J941" t="n">
-        <v>18.64999961853027</v>
+        <v>15.5</v>
       </c>
       <c r="K941" t="n">
         <v>0</v>
@@ -36330,7 +36330,7 @@
         <v>-2.439523969377792</v>
       </c>
       <c r="J942" t="n">
-        <v>18.64999961853027</v>
+        <v>15.5</v>
       </c>
       <c r="K942" t="n">
         <v>0</v>
@@ -36368,7 +36368,7 @@
         <v>-2.071428253537132</v>
       </c>
       <c r="J943" t="n">
-        <v>18.64999961853027</v>
+        <v>15.5</v>
       </c>
       <c r="K943" t="n">
         <v>0</v>
@@ -36406,13 +36406,13 @@
         <v>-0.9142858868553532</v>
       </c>
       <c r="J944" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K944" t="n">
-        <v>0</v>
+        <v>15.57999992370605</v>
       </c>
       <c r="L944" t="n">
-        <v>0</v>
+        <v>25.67391659108073</v>
       </c>
     </row>
     <row r="945">
@@ -36634,7 +36634,7 @@
         <v>-1.105714480082193</v>
       </c>
       <c r="J950" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K950" t="n">
         <v>0</v>
@@ -37166,7 +37166,7 @@
         <v>-1.084762209937686</v>
       </c>
       <c r="J964" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K964" t="n">
         <v>0</v>
@@ -37204,7 +37204,7 @@
         <v>-1.036190078372048</v>
       </c>
       <c r="J965" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K965" t="n">
         <v>0</v>
@@ -37242,7 +37242,7 @@
         <v>-0.9704760142735065</v>
       </c>
       <c r="J966" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K966" t="n">
         <v>0</v>
@@ -37280,7 +37280,7 @@
         <v>-1.212856883094425</v>
       </c>
       <c r="J967" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K967" t="n">
         <v>0</v>
@@ -37318,7 +37318,7 @@
         <v>-0.9190478097824819</v>
       </c>
       <c r="J968" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K968" t="n">
         <v>0</v>
@@ -38458,7 +38458,7 @@
         <v>-0.7952383586338581</v>
       </c>
       <c r="J998" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K998" t="n">
         <v>0</v>
@@ -39180,7 +39180,7 @@
         <v>-0.84857127780006</v>
       </c>
       <c r="J1017" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1017" t="n">
         <v>0</v>
@@ -39218,7 +39218,7 @@
         <v>-0.8766667048136387</v>
       </c>
       <c r="J1018" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1018" t="n">
         <v>0</v>
@@ -39256,7 +39256,7 @@
         <v>-1.048094885689872</v>
       </c>
       <c r="J1019" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1019" t="n">
         <v>0</v>
@@ -39294,7 +39294,7 @@
         <v>-0.9533334913707918</v>
       </c>
       <c r="J1020" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1020" t="n">
         <v>0</v>
@@ -39332,7 +39332,7 @@
         <v>-1.663809413001651</v>
       </c>
       <c r="J1021" t="n">
-        <v>18.64999961853027</v>
+        <v>13.59000015258789</v>
       </c>
       <c r="K1021" t="n">
         <v>0</v>
@@ -39370,13 +39370,13 @@
         <v>-0.9880954651605514</v>
       </c>
       <c r="J1022" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1022" t="n">
-        <v>0</v>
+        <v>14.19999980926514</v>
       </c>
       <c r="L1022" t="n">
-        <v>0</v>
+        <v>214.7886143911203</v>
       </c>
     </row>
     <row r="1023">
@@ -39408,7 +39408,7 @@
         <v>-1.387142862592425</v>
       </c>
       <c r="J1023" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1023" t="n">
         <v>0</v>
@@ -39446,7 +39446,7 @@
         <v>-1.810476393926711</v>
       </c>
       <c r="J1024" t="n">
-        <v>18.64999961853027</v>
+        <v>13.15999984741211</v>
       </c>
       <c r="K1024" t="n">
         <v>0</v>
@@ -39484,13 +39484,13 @@
         <v>-1.263809204101562</v>
       </c>
       <c r="J1025" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1025" t="n">
-        <v>0</v>
+        <v>13.60000038146973</v>
       </c>
       <c r="L1025" t="n">
-        <v>0</v>
+        <v>161.764897689682</v>
       </c>
     </row>
     <row r="1026">
@@ -39522,7 +39522,7 @@
         <v>-1.727619125729515</v>
       </c>
       <c r="J1026" t="n">
-        <v>18.64999961853027</v>
+        <v>13</v>
       </c>
       <c r="K1026" t="n">
         <v>0</v>
@@ -39560,13 +39560,13 @@
         <v>-0.9747621445428756</v>
       </c>
       <c r="J1027" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1027" t="n">
-        <v>0</v>
+        <v>13.65999984741211</v>
       </c>
       <c r="L1027" t="n">
-        <v>0</v>
+        <v>241.581205997285</v>
       </c>
     </row>
     <row r="1028">
@@ -39598,7 +39598,7 @@
         <v>-0.9528575170607798</v>
       </c>
       <c r="J1028" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1028" t="n">
         <v>0</v>
@@ -39636,7 +39636,7 @@
         <v>-0.9185719262985952</v>
       </c>
       <c r="J1029" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1029" t="n">
         <v>0</v>
@@ -41004,7 +41004,7 @@
         <v>-1.181905110677084</v>
       </c>
       <c r="J1065" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1065" t="n">
         <v>0</v>
@@ -41080,7 +41080,7 @@
         <v>-0.8995240983508879</v>
       </c>
       <c r="J1067" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1067" t="n">
         <v>0</v>
@@ -41118,7 +41118,7 @@
         <v>-0.7909525008428666</v>
       </c>
       <c r="J1068" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1068" t="n">
         <v>0</v>
@@ -41308,7 +41308,7 @@
         <v>-0.8466669264293856</v>
       </c>
       <c r="J1073" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1073" t="n">
         <v>0</v>
@@ -41346,7 +41346,7 @@
         <v>-1.197618938627697</v>
       </c>
       <c r="J1074" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1074" t="n">
         <v>0</v>
@@ -41384,7 +41384,7 @@
         <v>-1.273809750874838</v>
       </c>
       <c r="J1075" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1075" t="n">
         <v>0</v>
@@ -41422,7 +41422,7 @@
         <v>-1.017618769691104</v>
       </c>
       <c r="J1076" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1076" t="n">
         <v>0</v>
@@ -41460,7 +41460,7 @@
         <v>-0.8385710489182241</v>
       </c>
       <c r="J1077" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1077" t="n">
         <v>0</v>
@@ -41498,7 +41498,7 @@
         <v>-0.7957139242263072</v>
       </c>
       <c r="J1078" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1078" t="n">
         <v>0</v>
@@ -41536,7 +41536,7 @@
         <v>-1.045238131568546</v>
       </c>
       <c r="J1079" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1079" t="n">
         <v>0</v>
@@ -41574,7 +41574,7 @@
         <v>-0.9852378936040971</v>
       </c>
       <c r="J1080" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1080" t="n">
         <v>0</v>
@@ -41612,7 +41612,7 @@
         <v>-0.8814281736101428</v>
       </c>
       <c r="J1081" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1081" t="n">
         <v>0</v>
@@ -41802,7 +41802,7 @@
         <v>-0.8690478461129327</v>
       </c>
       <c r="J1086" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1086" t="n">
         <v>0</v>
@@ -41840,7 +41840,7 @@
         <v>-0.7957142875308083</v>
       </c>
       <c r="J1087" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1087" t="n">
         <v>0</v>
@@ -41878,7 +41878,7 @@
         <v>-1.152381261189779</v>
       </c>
       <c r="J1088" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1088" t="n">
         <v>0</v>
@@ -41916,7 +41916,7 @@
         <v>-1.284285363696871</v>
       </c>
       <c r="J1089" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1089" t="n">
         <v>0</v>
@@ -41954,7 +41954,7 @@
         <v>-0.7885714485531761</v>
       </c>
       <c r="J1090" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1090" t="n">
         <v>0</v>
@@ -41992,7 +41992,7 @@
         <v>-0.8123806544712604</v>
       </c>
       <c r="J1091" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1091" t="n">
         <v>0</v>
@@ -45868,7 +45868,7 @@
         <v>-1.24285670689174</v>
       </c>
       <c r="J1193" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1193" t="n">
         <v>0</v>
@@ -45906,7 +45906,7 @@
         <v>-1.205713907877605</v>
       </c>
       <c r="J1194" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1194" t="n">
         <v>0</v>
@@ -46286,7 +46286,7 @@
         <v>-0.9361906505766378</v>
       </c>
       <c r="J1204" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1204" t="n">
         <v>0</v>
@@ -46324,7 +46324,7 @@
         <v>-0.8138095310756128</v>
       </c>
       <c r="J1205" t="n">
-        <v>18.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1205" t="n">
         <v>0</v>
@@ -47771,10 +47771,10 @@
         <v>0</v>
       </c>
       <c r="K1243" t="n">
-        <v>19.34000015258789</v>
+        <v>0</v>
       </c>
       <c r="L1243" t="n">
-        <v>178.386899848418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1244">
@@ -49440,7 +49440,7 @@
         <v>-0.7876194545200903</v>
       </c>
       <c r="J1287" t="n">
-        <v>20.89999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1287" t="n">
         <v>0</v>
@@ -49478,7 +49478,7 @@
         <v>-0.939524695986794</v>
       </c>
       <c r="J1288" t="n">
-        <v>20.89999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1288" t="n">
         <v>0</v>
@@ -49516,7 +49516,7 @@
         <v>-1.186667396908714</v>
       </c>
       <c r="J1289" t="n">
-        <v>20.89999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1289" t="n">
         <v>0</v>
@@ -49557,10 +49557,10 @@
         <v>0</v>
       </c>
       <c r="K1290" t="n">
-        <v>21.14999961853027</v>
+        <v>0</v>
       </c>
       <c r="L1290" t="n">
-        <v>59.10165591231643</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1291">
@@ -49630,7 +49630,7 @@
         <v>-0.9266658964611239</v>
       </c>
       <c r="J1292" t="n">
-        <v>20.53000068664551</v>
+        <v>0</v>
       </c>
       <c r="K1292" t="n">
         <v>0</v>
@@ -49671,10 +49671,10 @@
         <v>0</v>
       </c>
       <c r="K1293" t="n">
-        <v>21.39999961853027</v>
+        <v>0</v>
       </c>
       <c r="L1293" t="n">
-        <v>203.2707821011905</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1294">
@@ -50808,7 +50808,7 @@
         <v>-0.8414280301048649</v>
       </c>
       <c r="J1323" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1323" t="n">
         <v>0</v>
@@ -50846,7 +50846,7 @@
         <v>-3.92095238821847</v>
       </c>
       <c r="J1324" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1324" t="n">
         <v>0</v>
@@ -50884,7 +50884,7 @@
         <v>-4.109048298427037</v>
       </c>
       <c r="J1325" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1325" t="n">
         <v>0</v>
@@ -50922,7 +50922,7 @@
         <v>-6.726666768391926</v>
       </c>
       <c r="J1326" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1326" t="n">
         <v>0</v>
@@ -50960,7 +50960,7 @@
         <v>-4.174286433628627</v>
       </c>
       <c r="J1327" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1327" t="n">
         <v>0</v>
@@ -50998,7 +50998,7 @@
         <v>-4.30428613935198</v>
       </c>
       <c r="J1328" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1328" t="n">
         <v>0</v>
@@ -51036,7 +51036,7 @@
         <v>-6.817619142078218</v>
       </c>
       <c r="J1329" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1329" t="n">
         <v>0</v>
@@ -51074,7 +51074,7 @@
         <v>-5.213332584926061</v>
       </c>
       <c r="J1330" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1330" t="n">
         <v>0</v>
@@ -51112,7 +51112,7 @@
         <v>-5.882856913975306</v>
       </c>
       <c r="J1331" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1331" t="n">
         <v>0</v>
@@ -51150,7 +51150,7 @@
         <v>-5.841904776436941</v>
       </c>
       <c r="J1332" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1332" t="n">
         <v>0</v>
@@ -51188,7 +51188,7 @@
         <v>-6.071428298950195</v>
       </c>
       <c r="J1333" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1333" t="n">
         <v>0</v>
@@ -51226,7 +51226,7 @@
         <v>-6.127618971325102</v>
       </c>
       <c r="J1334" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1334" t="n">
         <v>0</v>
@@ -51264,7 +51264,7 @@
         <v>-5.475238164265949</v>
       </c>
       <c r="J1335" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1335" t="n">
         <v>0</v>
@@ -51302,7 +51302,7 @@
         <v>-4.9499998546782</v>
       </c>
       <c r="J1336" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1336" t="n">
         <v>0</v>
@@ -51340,7 +51340,7 @@
         <v>-4.712856973920548</v>
       </c>
       <c r="J1337" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1337" t="n">
         <v>0</v>
@@ -51378,7 +51378,7 @@
         <v>-4.226189976646786</v>
       </c>
       <c r="J1338" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1338" t="n">
         <v>0</v>
@@ -51416,7 +51416,7 @@
         <v>-3.764761561439151</v>
       </c>
       <c r="J1339" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1339" t="n">
         <v>0</v>
@@ -51454,7 +51454,7 @@
         <v>-3.689523696899414</v>
       </c>
       <c r="J1340" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1340" t="n">
         <v>0</v>
@@ -51492,7 +51492,7 @@
         <v>-2.28238078526088</v>
       </c>
       <c r="J1341" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1341" t="n">
         <v>0</v>
@@ -51530,7 +51530,7 @@
         <v>-1.071429388863699</v>
       </c>
       <c r="J1342" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1342" t="n">
         <v>0</v>
@@ -51568,7 +51568,7 @@
         <v>-1.723809106009348</v>
       </c>
       <c r="J1343" t="n">
-        <v>23.27000045776367</v>
+        <v>20.07999992370605</v>
       </c>
       <c r="K1343" t="n">
         <v>0</v>
@@ -51606,7 +51606,7 @@
         <v>-1.325238364083425</v>
       </c>
       <c r="J1344" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1344" t="n">
         <v>0</v>
@@ -52673,10 +52673,10 @@
         <v>0</v>
       </c>
       <c r="K1372" t="n">
-        <v>0</v>
+        <v>20.40999984741211</v>
       </c>
       <c r="L1372" t="n">
-        <v>0</v>
+        <v>80.84270606888248</v>
       </c>
     </row>
     <row r="1373">
@@ -53050,7 +53050,7 @@
         <v>-0.8942849295479895</v>
       </c>
       <c r="J1382" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1382" t="n">
         <v>0</v>
@@ -53088,7 +53088,7 @@
         <v>-1.387143725440616</v>
       </c>
       <c r="J1383" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1383" t="n">
         <v>0</v>
@@ -53126,7 +53126,7 @@
         <v>-1.442856470743816</v>
       </c>
       <c r="J1384" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1384" t="n">
         <v>0</v>
@@ -53164,7 +53164,7 @@
         <v>-2.009524390811013</v>
       </c>
       <c r="J1385" t="n">
-        <v>23.27000045776367</v>
+        <v>17.71999931335449</v>
       </c>
       <c r="K1385" t="n">
         <v>0</v>
@@ -53202,13 +53202,13 @@
         <v>-1.317142395746139</v>
       </c>
       <c r="J1386" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1386" t="n">
-        <v>0</v>
+        <v>18.35000038146973</v>
       </c>
       <c r="L1386" t="n">
-        <v>0</v>
+        <v>171.6624128115618</v>
       </c>
     </row>
     <row r="1387">
@@ -53240,7 +53240,7 @@
         <v>-1.62142780848912</v>
       </c>
       <c r="J1387" t="n">
-        <v>23.27000045776367</v>
+        <v>17.95000076293945</v>
       </c>
       <c r="K1387" t="n">
         <v>0</v>
@@ -53278,13 +53278,13 @@
         <v>-1.21857216244652</v>
       </c>
       <c r="J1388" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1388" t="n">
-        <v>0</v>
+        <v>18.29999923706055</v>
       </c>
       <c r="L1388" t="n">
-        <v>0</v>
+        <v>95.62800238053795</v>
       </c>
     </row>
     <row r="1389">
@@ -53316,7 +53316,7 @@
         <v>-0.7580960591634103</v>
       </c>
       <c r="J1389" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1389" t="n">
         <v>0</v>
@@ -53354,7 +53354,7 @@
         <v>-1.044761476062593</v>
       </c>
       <c r="J1390" t="n">
-        <v>23.27000045776367</v>
+        <v>0</v>
       </c>
       <c r="K1390" t="n">
         <v>0</v>
@@ -54307,10 +54307,10 @@
         <v>0</v>
       </c>
       <c r="K1415" t="n">
-        <v>23.79000091552734</v>
+        <v>0</v>
       </c>
       <c r="L1415" t="n">
-        <v>109.2897094897285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1416">
@@ -55216,7 +55216,7 @@
         <v>-1.193809327625093</v>
       </c>
       <c r="J1439" t="n">
-        <v>25.35000038146973</v>
+        <v>0</v>
       </c>
       <c r="K1439" t="n">
         <v>0</v>
@@ -55254,7 +55254,7 @@
         <v>-1.019048690795898</v>
       </c>
       <c r="J1440" t="n">
-        <v>25.35000038146973</v>
+        <v>0</v>
       </c>
       <c r="K1440" t="n">
         <v>0</v>
@@ -55292,7 +55292,7 @@
         <v>-1.114762169974192</v>
       </c>
       <c r="J1441" t="n">
-        <v>25.35000038146973</v>
+        <v>0</v>
       </c>
       <c r="K1441" t="n">
         <v>0</v>
@@ -55330,7 +55330,7 @@
         <v>-2.154762268066406</v>
       </c>
       <c r="J1442" t="n">
-        <v>25.35000038146973</v>
+        <v>24.23999977111816</v>
       </c>
       <c r="K1442" t="n">
         <v>0</v>
@@ -55368,13 +55368,13 @@
         <v>-1.262856892177037</v>
       </c>
       <c r="J1443" t="n">
-        <v>25.35000038146973</v>
+        <v>0</v>
       </c>
       <c r="K1443" t="n">
-        <v>0</v>
+        <v>25.10000038146973</v>
       </c>
       <c r="L1443" t="n">
-        <v>0</v>
+        <v>171.3148600161904</v>
       </c>
     </row>
     <row r="1444">
@@ -55409,10 +55409,10 @@
         <v>0</v>
       </c>
       <c r="K1444" t="n">
-        <v>25.79999923706055</v>
+        <v>0</v>
       </c>
       <c r="L1444" t="n">
-        <v>87.20908311974232</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1445">
@@ -55482,7 +55482,7 @@
         <v>-1.101904732840403</v>
       </c>
       <c r="J1446" t="n">
-        <v>25.17000007629395</v>
+        <v>0</v>
       </c>
       <c r="K1446" t="n">
         <v>0</v>
@@ -55520,7 +55520,7 @@
         <v>-1.085238502139138</v>
       </c>
       <c r="J1447" t="n">
-        <v>25.17000007629395</v>
+        <v>0</v>
       </c>
       <c r="K1447" t="n">
         <v>0</v>
@@ -55558,7 +55558,7 @@
         <v>-1.762380145844958</v>
       </c>
       <c r="J1448" t="n">
-        <v>25.17000007629395</v>
+        <v>24.3700008392334</v>
       </c>
       <c r="K1448" t="n">
         <v>0</v>
@@ -55596,7 +55596,7 @@
         <v>-1.789523805890763</v>
       </c>
       <c r="J1449" t="n">
-        <v>25.17000007629395</v>
+        <v>24.3700008392334</v>
       </c>
       <c r="K1449" t="n">
         <v>0</v>
@@ -55640,7 +55640,7 @@
         <v>25.53000068664551</v>
       </c>
       <c r="L1450" t="n">
-        <v>70.50540553645094</v>
+        <v>227.1836694502899</v>
       </c>
     </row>
     <row r="1451">
@@ -55900,7 +55900,7 @@
         <v>-0.7757140568324488</v>
       </c>
       <c r="J1457" t="n">
-        <v>24.59000015258789</v>
+        <v>0</v>
       </c>
       <c r="K1457" t="n">
         <v>0</v>
@@ -55941,10 +55941,10 @@
         <v>0</v>
       </c>
       <c r="K1458" t="n">
-        <v>24.77000045776367</v>
+        <v>0</v>
       </c>
       <c r="L1458" t="n">
-        <v>36.33433626347868</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1459">
@@ -56090,7 +56090,7 @@
         <v>-1.459523246401833</v>
       </c>
       <c r="J1462" t="n">
-        <v>23.44000053405762</v>
+        <v>0</v>
       </c>
       <c r="K1462" t="n">
         <v>0</v>
@@ -56432,7 +56432,7 @@
         <v>-0.8838092258998316</v>
       </c>
       <c r="J1471" t="n">
-        <v>23.44000053405762</v>
+        <v>0</v>
       </c>
       <c r="K1471" t="n">
         <v>0</v>
@@ -59130,13 +59130,13 @@
         <v>-1.275714965093705</v>
       </c>
       <c r="J1542" t="n">
-        <v>25.82999992370605</v>
+        <v>0</v>
       </c>
       <c r="K1542" t="n">
-        <v>0</v>
+        <v>26.71999931335449</v>
       </c>
       <c r="L1542" t="n">
-        <v>0</v>
+        <v>166.5418062349315</v>
       </c>
     </row>
     <row r="1543">
@@ -59168,7 +59168,7 @@
         <v>-1.129047575451079</v>
       </c>
       <c r="J1543" t="n">
-        <v>25.82999992370605</v>
+        <v>0</v>
       </c>
       <c r="K1543" t="n">
         <v>0</v>
@@ -59209,10 +59209,10 @@
         <v>0</v>
       </c>
       <c r="K1544" t="n">
-        <v>27.60000038146973</v>
+        <v>0</v>
       </c>
       <c r="L1544" t="n">
-        <v>320.6522524093925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1545">
@@ -59510,7 +59510,7 @@
         <v>-0.8928577786400211</v>
       </c>
       <c r="J1552" t="n">
-        <v>26.72999954223633</v>
+        <v>0</v>
       </c>
       <c r="K1552" t="n">
         <v>0</v>
@@ -59551,10 +59551,10 @@
         <v>0</v>
       </c>
       <c r="K1553" t="n">
-        <v>26.85000038146973</v>
+        <v>0</v>
       </c>
       <c r="L1553" t="n">
-        <v>22.34652467942158</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1554">
@@ -59624,7 +59624,7 @@
         <v>-1.066666466849192</v>
       </c>
       <c r="J1555" t="n">
-        <v>26.35000038146973</v>
+        <v>0</v>
       </c>
       <c r="K1555" t="n">
         <v>0</v>
@@ -59665,10 +59665,10 @@
         <v>0</v>
       </c>
       <c r="K1556" t="n">
-        <v>27.3700008392334</v>
+        <v>0</v>
       </c>
       <c r="L1556" t="n">
-        <v>186.3354816382682</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1557">
@@ -59776,7 +59776,7 @@
         <v>-1.079048156738281</v>
       </c>
       <c r="J1559" t="n">
-        <v>25.89999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1559" t="n">
         <v>0</v>
@@ -59814,7 +59814,7 @@
         <v>-0.8838096800304598</v>
       </c>
       <c r="J1560" t="n">
-        <v>25.89999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1560" t="n">
         <v>0</v>
@@ -59852,7 +59852,7 @@
         <v>-1.00619143531436</v>
       </c>
       <c r="J1561" t="n">
-        <v>25.89999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1561" t="n">
         <v>0</v>
@@ -59890,7 +59890,7 @@
         <v>-1.584761574154808</v>
       </c>
       <c r="J1562" t="n">
-        <v>25.89999961853027</v>
+        <v>25.27000045776367</v>
       </c>
       <c r="K1562" t="n">
         <v>0</v>
@@ -59928,7 +59928,7 @@
         <v>-2.077618916829426</v>
       </c>
       <c r="J1563" t="n">
-        <v>25.89999961853027</v>
+        <v>25.27000045776367</v>
       </c>
       <c r="K1563" t="n">
         <v>0</v>
@@ -59966,13 +59966,13 @@
         <v>-1.179047357468377</v>
       </c>
       <c r="J1564" t="n">
-        <v>25.89999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1564" t="n">
-        <v>0</v>
+        <v>25.52000045776367</v>
       </c>
       <c r="L1564" t="n">
-        <v>0</v>
+        <v>48.98119034397298</v>
       </c>
     </row>
     <row r="1565">
@@ -60007,10 +60007,10 @@
         <v>0</v>
       </c>
       <c r="K1565" t="n">
-        <v>26.48999977111816</v>
+        <v>0</v>
       </c>
       <c r="L1565" t="n">
-        <v>111.3628081701917</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1566">
@@ -61752,7 +61752,7 @@
         <v>-1.353810083298455</v>
       </c>
       <c r="J1611" t="n">
-        <v>26.13999938964844</v>
+        <v>0</v>
       </c>
       <c r="K1611" t="n">
         <v>0</v>
@@ -61790,7 +61790,7 @@
         <v>-1.073334103538876</v>
       </c>
       <c r="J1612" t="n">
-        <v>26.13999938964844</v>
+        <v>0</v>
       </c>
       <c r="K1612" t="n">
         <v>0</v>
@@ -61828,7 +61828,7 @@
         <v>-1.157619203839982</v>
       </c>
       <c r="J1613" t="n">
-        <v>26.13999938964844</v>
+        <v>0</v>
       </c>
       <c r="K1613" t="n">
         <v>0</v>
@@ -61866,7 +61866,7 @@
         <v>-1.261428560529435</v>
       </c>
       <c r="J1614" t="n">
-        <v>26.13999938964844</v>
+        <v>0</v>
       </c>
       <c r="K1614" t="n">
         <v>0</v>
@@ -61904,7 +61904,7 @@
         <v>-1.064285641624814</v>
       </c>
       <c r="J1615" t="n">
-        <v>26.13999938964844</v>
+        <v>0</v>
       </c>
       <c r="K1615" t="n">
         <v>0</v>
@@ -61942,7 +61942,7 @@
         <v>-0.7628566196986597</v>
       </c>
       <c r="J1616" t="n">
-        <v>26.13999938964844</v>
+        <v>0</v>
       </c>
       <c r="K1616" t="n">
         <v>0</v>
@@ -61980,7 +61980,7 @@
         <v>-1.645238785516646</v>
       </c>
       <c r="J1617" t="n">
-        <v>26.13999938964844</v>
+        <v>25.54999923706055</v>
       </c>
       <c r="K1617" t="n">
         <v>0</v>
@@ -62018,13 +62018,13 @@
         <v>-1.24285788763137</v>
       </c>
       <c r="J1618" t="n">
-        <v>26.13999938964844</v>
+        <v>0</v>
       </c>
       <c r="K1618" t="n">
-        <v>0</v>
+        <v>25.8799991607666</v>
       </c>
       <c r="L1618" t="n">
-        <v>0</v>
+        <v>63.75578330897435</v>
       </c>
     </row>
     <row r="1619">
@@ -62056,7 +62056,7 @@
         <v>-1.425237655639648</v>
       </c>
       <c r="J1619" t="n">
-        <v>26.13999938964844</v>
+        <v>0</v>
       </c>
       <c r="K1619" t="n">
         <v>0</v>
@@ -62097,10 +62097,10 @@
         <v>0</v>
       </c>
       <c r="K1620" t="n">
-        <v>26.35000038146973</v>
+        <v>0</v>
       </c>
       <c r="L1620" t="n">
-        <v>39.84838496795039</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1621">
@@ -62170,7 +62170,7 @@
         <v>-1.055238451276505</v>
       </c>
       <c r="J1622" t="n">
-        <v>25.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1622" t="n">
         <v>0</v>
@@ -62208,7 +62208,7 @@
         <v>-0.8014276595342729</v>
       </c>
       <c r="J1623" t="n">
-        <v>25.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1623" t="n">
         <v>0</v>
@@ -62246,7 +62246,7 @@
         <v>-1.532857077462332</v>
       </c>
       <c r="J1624" t="n">
-        <v>25.64999961853027</v>
+        <v>24.92000007629395</v>
       </c>
       <c r="K1624" t="n">
         <v>0</v>
@@ -62284,7 +62284,7 @@
         <v>-2.058571860903786</v>
       </c>
       <c r="J1625" t="n">
-        <v>25.64999961853027</v>
+        <v>24.92000007629395</v>
       </c>
       <c r="K1625" t="n">
         <v>0</v>
@@ -62322,7 +62322,7 @@
         <v>-2.207142966134207</v>
       </c>
       <c r="J1626" t="n">
-        <v>25.64999961853027</v>
+        <v>24.92000007629395</v>
       </c>
       <c r="K1626" t="n">
         <v>0</v>
@@ -62360,7 +62360,7 @@
         <v>-1.924761181785946</v>
       </c>
       <c r="J1627" t="n">
-        <v>25.64999961853027</v>
+        <v>24.92000007629395</v>
       </c>
       <c r="K1627" t="n">
         <v>0</v>
@@ -62398,7 +62398,7 @@
         <v>-1.769523348127091</v>
       </c>
       <c r="J1628" t="n">
-        <v>25.64999961853027</v>
+        <v>24.92000007629395</v>
       </c>
       <c r="K1628" t="n">
         <v>0</v>
@@ -62439,10 +62439,10 @@
         <v>0</v>
       </c>
       <c r="K1629" t="n">
-        <v>0</v>
+        <v>25.45000076293945</v>
       </c>
       <c r="L1629" t="n">
-        <v>0</v>
+        <v>104.1258685181063</v>
       </c>
     </row>
     <row r="1630">
@@ -62512,7 +62512,7 @@
         <v>-1.185237430390856</v>
       </c>
       <c r="J1631" t="n">
-        <v>25.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1631" t="n">
         <v>0</v>
@@ -62550,7 +62550,7 @@
         <v>-1.401429494222004</v>
       </c>
       <c r="J1632" t="n">
-        <v>25.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1632" t="n">
         <v>0</v>
@@ -62588,7 +62588,7 @@
         <v>-0.9242856161934974</v>
       </c>
       <c r="J1633" t="n">
-        <v>25.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="K1633" t="n">
         <v>0</v>
@@ -62819,10 +62819,10 @@
         <v>0</v>
       </c>
       <c r="K1639" t="n">
-        <v>26.26000022888184</v>
+        <v>0</v>
       </c>
       <c r="L1639" t="n">
-        <v>116.1463452084548</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1640">
@@ -63690,7 +63690,7 @@
         <v>-1.008571352277482</v>
       </c>
       <c r="J1662" t="n">
-        <v>26.17000007629395</v>
+        <v>0</v>
       </c>
       <c r="K1662" t="n">
         <v>0</v>
@@ -63728,7 +63728,7 @@
         <v>-1.115237644740514</v>
       </c>
       <c r="J1663" t="n">
-        <v>26.17000007629395</v>
+        <v>0</v>
       </c>
       <c r="K1663" t="n">
         <v>0</v>
@@ -63769,10 +63769,10 @@
         <v>0</v>
       </c>
       <c r="K1664" t="n">
-        <v>26.52000045776367</v>
+        <v>0</v>
       </c>
       <c r="L1664" t="n">
-        <v>65.98800441710866</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1665">
@@ -64830,7 +64830,7 @@
         <v>-0.8080945696149548</v>
       </c>
       <c r="J1692" t="n">
-        <v>28.78000068664551</v>
+        <v>0</v>
       </c>
       <c r="K1692" t="n">
         <v>0</v>
@@ -64871,10 +64871,10 @@
         <v>0</v>
       </c>
       <c r="K1693" t="n">
-        <v>29.85000038146973</v>
+        <v>0</v>
       </c>
       <c r="L1693" t="n">
-        <v>179.2294273283247</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1694">
@@ -66198,7 +66198,7 @@
         <v>-0.8038103921072839</v>
       </c>
       <c r="J1728" t="n">
-        <v>29.54999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1728" t="n">
         <v>0</v>
@@ -66236,7 +66236,7 @@
         <v>-0.7647616068522147</v>
       </c>
       <c r="J1729" t="n">
-        <v>29.54999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1729" t="n">
         <v>0</v>
@@ -66277,10 +66277,10 @@
         <v>0</v>
       </c>
       <c r="K1730" t="n">
-        <v>29.85000038146973</v>
+        <v>0</v>
       </c>
       <c r="L1730" t="n">
-        <v>50.25144733254582</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1731">
@@ -66388,7 +66388,7 @@
         <v>-0.9461897895449667</v>
       </c>
       <c r="J1733" t="n">
-        <v>29.29000091552734</v>
+        <v>0</v>
       </c>
       <c r="K1733" t="n">
         <v>0</v>
@@ -66429,10 +66429,10 @@
         <v>0</v>
       </c>
       <c r="K1734" t="n">
-        <v>29.64999961853027</v>
+        <v>0</v>
       </c>
       <c r="L1734" t="n">
-        <v>60.70804513230792</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1735">
@@ -66464,7 +66464,7 @@
         <v>-0.8447628021240234</v>
       </c>
       <c r="J1735" t="n">
-        <v>29.29999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1735" t="n">
         <v>0</v>
@@ -66502,7 +66502,7 @@
         <v>-1.997142337617419</v>
       </c>
       <c r="J1736" t="n">
-        <v>29.29999923706055</v>
+        <v>28.03000068664551</v>
       </c>
       <c r="K1736" t="n">
         <v>0</v>
@@ -66540,13 +66540,13 @@
         <v>-1.12666756766183</v>
       </c>
       <c r="J1737" t="n">
-        <v>29.29999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1737" t="n">
-        <v>0</v>
+        <v>28.79999923706055</v>
       </c>
       <c r="L1737" t="n">
-        <v>0</v>
+        <v>133.6803074328186</v>
       </c>
     </row>
     <row r="1738">
@@ -66578,7 +66578,7 @@
         <v>-0.9971426100957963</v>
       </c>
       <c r="J1738" t="n">
-        <v>29.29999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1738" t="n">
         <v>0</v>
@@ -66616,7 +66616,7 @@
         <v>-0.8480948493594198</v>
       </c>
       <c r="J1739" t="n">
-        <v>29.29999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1739" t="n">
         <v>0</v>
@@ -66654,7 +66654,7 @@
         <v>-1.23095176333473</v>
       </c>
       <c r="J1740" t="n">
-        <v>29.29999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1740" t="n">
         <v>0</v>
@@ -66692,7 +66692,7 @@
         <v>-1.392856961204892</v>
       </c>
       <c r="J1741" t="n">
-        <v>29.29999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1741" t="n">
         <v>0</v>
@@ -66730,7 +66730,7 @@
         <v>-0.8390485672723678</v>
       </c>
       <c r="J1742" t="n">
-        <v>29.29999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1742" t="n">
         <v>0</v>
@@ -66768,7 +66768,7 @@
         <v>-0.9695244743710489</v>
       </c>
       <c r="J1743" t="n">
-        <v>29.29999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1743" t="n">
         <v>0</v>
@@ -66923,10 +66923,10 @@
         <v>0</v>
       </c>
       <c r="K1747" t="n">
-        <v>29.47999954223633</v>
+        <v>0</v>
       </c>
       <c r="L1747" t="n">
-        <v>30.52922455407314</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1748">
@@ -68174,7 +68174,7 @@
         <v>-1.056666465032668</v>
       </c>
       <c r="J1780" t="n">
-        <v>25.29999923706055</v>
+        <v>0</v>
       </c>
       <c r="K1780" t="n">
         <v>0</v>

</xml_diff>